<commit_message>
Updated BOM and pos files for v1.0
</commit_message>
<xml_diff>
--- a/rp2350b-launchpad-PCB-top-pos.xlsx
+++ b/rp2350b-launchpad-PCB-top-pos.xlsx
@@ -52,6 +52,63 @@
     <t xml:space="preserve">90.000000</t>
   </si>
   <si>
+    <t xml:space="preserve">C2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14.224000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">68.120500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">61.292500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32.232500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">78.740000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.000000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34.925000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">60.680500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">40.894000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">46.990000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-90.000000</t>
+  </si>
+  <si>
     <t xml:space="preserve">C10</t>
   </si>
   <si>
@@ -100,36 +157,18 @@
     <t xml:space="preserve">C16</t>
   </si>
   <si>
-    <t xml:space="preserve">60.680500</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-90.000000</t>
-  </si>
-  <si>
     <t xml:space="preserve">C17</t>
   </si>
   <si>
     <t xml:space="preserve">C18</t>
   </si>
   <si>
-    <t xml:space="preserve">46.990000</t>
-  </si>
-  <si>
     <t xml:space="preserve">C19</t>
   </si>
   <si>
     <t xml:space="preserve">36.322000</t>
   </si>
   <si>
-    <t xml:space="preserve">C2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14.224000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">68.120500</t>
-  </si>
-  <si>
     <t xml:space="preserve">C20</t>
   </si>
   <si>
@@ -145,9 +184,6 @@
     <t xml:space="preserve">16.637000</t>
   </si>
   <si>
-    <t xml:space="preserve">0.000000</t>
-  </si>
-  <si>
     <t xml:space="preserve">C22</t>
   </si>
   <si>
@@ -157,63 +193,57 @@
     <t xml:space="preserve">C23</t>
   </si>
   <si>
-    <t xml:space="preserve">25.400000</t>
+    <t xml:space="preserve">25.146000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25.781000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18.030000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24.257000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31.496000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">45.565000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.924000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18.034000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33.147000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C29</t>
   </si>
   <si>
     <t xml:space="preserve">25.908000</t>
   </si>
   <si>
-    <t xml:space="preserve">C24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18.030000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25.781000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22.733000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22.606000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">31.496000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">45.565000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26.924000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18.034000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">33.147000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C29</t>
-  </si>
-  <si>
     <t xml:space="preserve">43.561000</t>
   </si>
   <si>
-    <t xml:space="preserve">C3</t>
-  </si>
-  <si>
     <t xml:space="preserve">C30</t>
   </si>
   <si>
@@ -280,12 +310,6 @@
     <t xml:space="preserve">28.321000</t>
   </si>
   <si>
-    <t xml:space="preserve">C4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">61.292500</t>
-  </si>
-  <si>
     <t xml:space="preserve">C40</t>
   </si>
   <si>
@@ -295,33 +319,6 @@
     <t xml:space="preserve">21.943000</t>
   </si>
   <si>
-    <t xml:space="preserve">C5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">32.232500</t>
-  </si>
-  <si>
-    <t xml:space="preserve">78.740000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">34.925000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">40.894000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C9</t>
-  </si>
-  <si>
     <t xml:space="preserve">D1</t>
   </si>
   <si>
@@ -373,7 +370,10 @@
     <t xml:space="preserve">L2</t>
   </si>
   <si>
-    <t xml:space="preserve">23.046000</t>
+    <t xml:space="preserve">25.162000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22.352000</t>
   </si>
   <si>
     <t xml:space="preserve">R1</t>
@@ -382,6 +382,54 @@
     <t xml:space="preserve">71.755000</t>
   </si>
   <si>
+    <t xml:space="preserve">R2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.969000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28.727500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">75.756000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18.250000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">77.925000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.445000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">75.755000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22.225000</t>
+  </si>
+  <si>
     <t xml:space="preserve">R10</t>
   </si>
   <si>
@@ -397,9 +445,6 @@
     <t xml:space="preserve">R13</t>
   </si>
   <si>
-    <t xml:space="preserve">28.727500</t>
-  </si>
-  <si>
     <t xml:space="preserve">R14</t>
   </si>
   <si>
@@ -415,9 +460,6 @@
     <t xml:space="preserve">R17</t>
   </si>
   <si>
-    <t xml:space="preserve">22.225000</t>
-  </si>
-  <si>
     <t xml:space="preserve">7.620000</t>
   </si>
   <si>
@@ -430,15 +472,9 @@
     <t xml:space="preserve">R19</t>
   </si>
   <si>
-    <t xml:space="preserve">5.969000</t>
-  </si>
-  <si>
     <t xml:space="preserve">5.525000</t>
   </si>
   <si>
-    <t xml:space="preserve">R2</t>
-  </si>
-  <si>
     <t xml:space="preserve">R20</t>
   </si>
   <si>
@@ -508,9 +544,6 @@
     <t xml:space="preserve">36.195000</t>
   </si>
   <si>
-    <t xml:space="preserve">R3</t>
-  </si>
-  <si>
     <t xml:space="preserve">R30</t>
   </si>
   <si>
@@ -538,39 +571,6 @@
     <t xml:space="preserve">13.970000</t>
   </si>
   <si>
-    <t xml:space="preserve">R4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">75.756000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18.250000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">77.925000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.445000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">75.755000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R9</t>
-  </si>
-  <si>
     <t xml:space="preserve">S1</t>
   </si>
   <si>
@@ -622,6 +622,63 @@
     <t xml:space="preserve">72.710000</t>
   </si>
   <si>
+    <t xml:space="preserve">U2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">68.133000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">61.280000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">75.184000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">41.148000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">68.580000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.279000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20.535000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33.159000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20.673000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29.210000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33.020000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U9</t>
+  </si>
+  <si>
     <t xml:space="preserve">U10</t>
   </si>
   <si>
@@ -656,63 +713,6 @@
   </si>
   <si>
     <t xml:space="preserve">U16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">68.133000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">61.280000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">75.184000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">41.148000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">68.580000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">37.279000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20.535000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">33.159000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20.673000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29.210000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">33.020000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U9</t>
   </si>
   <si>
     <t xml:space="preserve">USB1</t>
@@ -873,19 +873,19 @@
   </sheetPr>
   <dimension ref="A1:I107"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G31" activeCellId="0" sqref="G31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2:E107"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="5.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="5.16"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -946,7 +946,7 @@
         <v>13</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>12</v>
@@ -961,13 +961,13 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>15</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>12</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>8</v>
@@ -979,13 +979,13 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>8</v>
@@ -997,73 +997,73 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="D7" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>20</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>22</v>
       </c>
       <c r="I7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>24</v>
-      </c>
       <c r="D8" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="I8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="0" t="s">
-        <v>16</v>
-      </c>
       <c r="C9" s="0" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="I9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="0" t="s">
         <v>28</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>27</v>
       </c>
       <c r="I10" s="1"/>
     </row>
@@ -1075,7 +1075,7 @@
         <v>30</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>8</v>
@@ -1087,13 +1087,13 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="0" t="s">
         <v>31</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>12</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>8</v>
@@ -1105,13 +1105,13 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>8</v>
@@ -1129,7 +1129,7 @@
         <v>37</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>8</v>
@@ -1162,16 +1162,16 @@
         <v>42</v>
       </c>
       <c r="B16" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="0" t="s">
-        <v>40</v>
-      </c>
       <c r="D16" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="I16" s="1"/>
     </row>
@@ -1180,154 +1180,154 @@
         <v>44</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="I17" s="1"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="I18" s="1"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="I19" s="1"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="D20" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="I20" s="1"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="D21" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="I21" s="1"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D22" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I22" s="1"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="D23" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="I23" s="1"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>6</v>
+        <v>57</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="D24" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="I24" s="1"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D25" s="0" t="s">
         <v>8</v>
@@ -1339,67 +1339,67 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D26" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="I26" s="1"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B27" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="C27" s="0" t="s">
-        <v>70</v>
-      </c>
       <c r="D27" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="I27" s="1"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B28" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="C28" s="0" t="s">
-        <v>72</v>
-      </c>
       <c r="D28" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="I28" s="1"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D29" s="0" t="s">
         <v>8</v>
@@ -1411,136 +1411,136 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D30" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="I30" s="1"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D31" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I31" s="1"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D32" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="I32" s="1"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D33" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I33" s="1"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D34" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I34" s="1"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>6</v>
+        <v>84</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D35" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="I35" s="1"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D36" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="I36" s="1"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>34</v>
+        <v>89</v>
       </c>
       <c r="C37" s="0" t="s">
         <v>87</v>
@@ -1549,19 +1549,19 @@
         <v>8</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="I37" s="1"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D38" s="0" t="s">
         <v>8</v>
@@ -1573,190 +1573,190 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>26</v>
+        <v>93</v>
       </c>
       <c r="D39" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="I39" s="1"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>98</v>
+        <v>69</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>26</v>
+        <v>95</v>
       </c>
       <c r="D40" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="I40" s="1"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>30</v>
+        <v>97</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>26</v>
+        <v>98</v>
       </c>
       <c r="D41" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I41" s="1"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="B42" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="B42" s="0" t="s">
+      <c r="C42" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="C42" s="0" t="s">
-        <v>102</v>
-      </c>
       <c r="D42" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="I42" s="1"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C43" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="B43" s="0" t="s">
+      <c r="D43" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E43" s="0" t="s">
         <v>20</v>
-      </c>
-      <c r="C43" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="D43" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E43" s="0" t="s">
-        <v>41</v>
       </c>
       <c r="I43" s="1"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C44" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="B44" s="0" t="s">
+      <c r="D44" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E44" s="0" t="s">
         <v>20</v>
-      </c>
-      <c r="C44" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="D44" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E44" s="0" t="s">
-        <v>41</v>
       </c>
       <c r="I44" s="1"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C45" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="B45" s="0" t="s">
+      <c r="D45" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E45" s="0" t="s">
         <v>20</v>
-      </c>
-      <c r="C45" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="D45" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E45" s="0" t="s">
-        <v>41</v>
       </c>
       <c r="I45" s="1"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C46" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="B46" s="0" t="s">
+      <c r="D46" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E46" s="0" t="s">
         <v>20</v>
-      </c>
-      <c r="C46" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="D46" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E46" s="0" t="s">
-        <v>41</v>
       </c>
       <c r="I46" s="1"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="B47" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="B47" s="0" t="s">
+      <c r="C47" s="0" t="s">
         <v>112</v>
       </c>
-      <c r="C47" s="0" t="s">
-        <v>113</v>
-      </c>
       <c r="D47" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I47" s="1"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="B48" s="0" t="s">
         <v>114</v>
       </c>
-      <c r="B48" s="0" t="s">
-        <v>115</v>
-      </c>
       <c r="C48" s="0" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D48" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="I48" s="1"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="B49" s="0" t="s">
         <v>116</v>
-      </c>
-      <c r="B49" s="0" t="s">
-        <v>45</v>
       </c>
       <c r="C49" s="0" t="s">
         <v>117</v>
@@ -1765,7 +1765,7 @@
         <v>8</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="I49" s="1"/>
     </row>
@@ -1774,7 +1774,7 @@
         <v>118</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C50" s="0" t="s">
         <v>119</v>
@@ -1783,7 +1783,7 @@
         <v>8</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="I50" s="1"/>
     </row>
@@ -1792,10 +1792,10 @@
         <v>120</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>98</v>
+        <v>121</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D51" s="0" t="s">
         <v>8</v>
@@ -1807,19 +1807,19 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>122</v>
+        <v>100</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>12</v>
+        <v>105</v>
       </c>
       <c r="D52" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="I52" s="1"/>
     </row>
@@ -1828,16 +1828,16 @@
         <v>123</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>14</v>
+        <v>100</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>26</v>
+        <v>107</v>
       </c>
       <c r="D53" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="I53" s="1"/>
     </row>
@@ -1849,13 +1849,13 @@
         <v>125</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="D54" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="I54" s="1"/>
     </row>
@@ -1864,16 +1864,16 @@
         <v>126</v>
       </c>
       <c r="B55" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="C55" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="C55" s="0" t="s">
-        <v>106</v>
-      </c>
       <c r="D55" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="I55" s="1"/>
     </row>
@@ -1882,100 +1882,100 @@
         <v>128</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>108</v>
+        <v>130</v>
       </c>
       <c r="D56" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="I56" s="1"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>110</v>
+        <v>133</v>
       </c>
       <c r="D57" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="I57" s="1"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>132</v>
+        <v>31</v>
       </c>
       <c r="D58" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="I58" s="1"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>134</v>
+        <v>25</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>75</v>
+        <v>31</v>
       </c>
       <c r="D59" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="I59" s="1"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>137</v>
+        <v>31</v>
       </c>
       <c r="D60" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="I60" s="1"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>136</v>
+        <v>33</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="D61" s="0" t="s">
         <v>8</v>
@@ -1987,19 +1987,19 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>137</v>
+        <v>19</v>
       </c>
       <c r="D62" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="I62" s="1"/>
     </row>
@@ -2008,286 +2008,286 @@
         <v>141</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>57</v>
+        <v>142</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>68</v>
+        <v>105</v>
       </c>
       <c r="D63" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="I63" s="1"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>144</v>
+        <v>107</v>
       </c>
       <c r="D64" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="I64" s="1"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>147</v>
+        <v>109</v>
       </c>
       <c r="D65" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="I65" s="1"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>74</v>
+        <v>135</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>49</v>
+        <v>146</v>
       </c>
       <c r="D66" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="I66" s="1"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="D67" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="I67" s="1"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>152</v>
+        <v>121</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D68" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I68" s="1"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D69" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="I69" s="1"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>158</v>
+        <v>78</v>
       </c>
       <c r="D70" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="I70" s="1"/>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="D71" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="I71" s="1"/>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>101</v>
+        <v>158</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>106</v>
+        <v>159</v>
       </c>
       <c r="D72" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E72" s="0" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="I72" s="1"/>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>164</v>
+        <v>58</v>
       </c>
       <c r="D73" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E73" s="0" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="I73" s="1"/>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>167</v>
+        <v>58</v>
       </c>
       <c r="D74" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E74" s="0" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="I74" s="1"/>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D75" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E75" s="0" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="I75" s="1"/>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>113</v>
+        <v>168</v>
       </c>
       <c r="D76" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E76" s="0" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="I76" s="1"/>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>108</v>
+        <v>170</v>
       </c>
       <c r="D77" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E77" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I77" s="1"/>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="B78" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C78" s="0" t="s">
         <v>173</v>
       </c>
-      <c r="B78" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="C78" s="0" t="s">
-        <v>104</v>
-      </c>
       <c r="D78" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E78" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I78" s="1"/>
     </row>
@@ -2296,7 +2296,7 @@
         <v>174</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>136</v>
+        <v>84</v>
       </c>
       <c r="C79" s="0" t="s">
         <v>175</v>
@@ -2305,7 +2305,7 @@
         <v>8</v>
       </c>
       <c r="E79" s="0" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="I79" s="1"/>
     </row>
@@ -2323,7 +2323,7 @@
         <v>8</v>
       </c>
       <c r="E80" s="0" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="I80" s="1"/>
     </row>
@@ -2335,31 +2335,31 @@
         <v>180</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D81" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E81" s="0" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="I81" s="1"/>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="B82" s="0" t="s">
         <v>182</v>
       </c>
-      <c r="B82" s="0" t="s">
-        <v>131</v>
-      </c>
       <c r="C82" s="0" t="s">
-        <v>12</v>
+        <v>112</v>
       </c>
       <c r="D82" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E82" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I82" s="1"/>
     </row>
@@ -2377,7 +2377,7 @@
         <v>8</v>
       </c>
       <c r="E83" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I83" s="1"/>
     </row>
@@ -2413,7 +2413,7 @@
         <v>8</v>
       </c>
       <c r="E85" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I85" s="1"/>
     </row>
@@ -2431,7 +2431,7 @@
         <v>8</v>
       </c>
       <c r="E86" s="0" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="I86" s="1"/>
     </row>
@@ -2449,7 +2449,7 @@
         <v>8</v>
       </c>
       <c r="E87" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I87" s="1"/>
     </row>
@@ -2467,7 +2467,7 @@
         <v>8</v>
       </c>
       <c r="E88" s="0" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="I88" s="1"/>
     </row>
@@ -2476,16 +2476,16 @@
         <v>200</v>
       </c>
       <c r="B89" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="C89" s="0" t="s">
         <v>201</v>
       </c>
-      <c r="C89" s="0" t="s">
-        <v>113</v>
-      </c>
       <c r="D89" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E89" s="0" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="I89" s="1"/>
     </row>
@@ -2494,16 +2494,16 @@
         <v>202</v>
       </c>
       <c r="B90" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="C90" s="0" t="s">
         <v>203</v>
       </c>
-      <c r="C90" s="0" t="s">
-        <v>113</v>
-      </c>
       <c r="D90" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E90" s="0" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="I90" s="1"/>
     </row>
@@ -2512,16 +2512,16 @@
         <v>204</v>
       </c>
       <c r="B91" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C91" s="0" t="s">
         <v>205</v>
       </c>
-      <c r="C91" s="0" t="s">
-        <v>113</v>
-      </c>
       <c r="D91" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E91" s="0" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="I91" s="1"/>
     </row>
@@ -2530,196 +2530,196 @@
         <v>206</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>122</v>
+        <v>207</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>113</v>
+        <v>208</v>
       </c>
       <c r="D92" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E92" s="0" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="I92" s="1"/>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>113</v>
+        <v>211</v>
       </c>
       <c r="D93" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E93" s="0" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="I93" s="1"/>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>113</v>
+        <v>214</v>
       </c>
       <c r="D94" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E94" s="0" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="I94" s="1"/>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>30</v>
+        <v>216</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>113</v>
+        <v>217</v>
       </c>
       <c r="D95" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E95" s="0" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="I95" s="1"/>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>198</v>
+        <v>216</v>
       </c>
       <c r="C96" s="0" t="s">
-        <v>213</v>
+        <v>112</v>
       </c>
       <c r="D96" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E96" s="0" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="I96" s="1"/>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>198</v>
+        <v>220</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>215</v>
+        <v>112</v>
       </c>
       <c r="D97" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E97" s="0" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="I97" s="1"/>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="B98" s="0" t="s">
-        <v>72</v>
+        <v>222</v>
       </c>
       <c r="C98" s="0" t="s">
-        <v>217</v>
+        <v>112</v>
       </c>
       <c r="D98" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E98" s="0" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="I98" s="1"/>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="B99" s="0" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="C99" s="0" t="s">
-        <v>220</v>
+        <v>112</v>
       </c>
       <c r="D99" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E99" s="0" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="I99" s="1"/>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="B100" s="0" t="s">
-        <v>222</v>
+        <v>138</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>223</v>
+        <v>112</v>
       </c>
       <c r="D100" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E100" s="0" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="I100" s="1"/>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B101" s="0" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="C101" s="0" t="s">
-        <v>226</v>
+        <v>112</v>
       </c>
       <c r="D101" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E101" s="0" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="I101" s="1"/>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B102" s="0" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>229</v>
+        <v>112</v>
       </c>
       <c r="D102" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E102" s="0" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="I102" s="1"/>
     </row>
@@ -2728,10 +2728,10 @@
         <v>230</v>
       </c>
       <c r="B103" s="0" t="s">
-        <v>228</v>
+        <v>27</v>
       </c>
       <c r="C103" s="0" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D103" s="0" t="s">
         <v>8</v>
@@ -2755,7 +2755,7 @@
         <v>8</v>
       </c>
       <c r="E104" s="0" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="I104" s="1"/>
     </row>
@@ -2773,7 +2773,7 @@
         <v>8</v>
       </c>
       <c r="E105" s="0" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="I105" s="1"/>
     </row>
@@ -2791,7 +2791,7 @@
         <v>8</v>
       </c>
       <c r="E106" s="0" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="I106" s="1"/>
     </row>
@@ -2800,7 +2800,7 @@
         <v>240</v>
       </c>
       <c r="B107" s="0" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="C107" s="0" t="s">
         <v>241</v>

</xml_diff>

<commit_message>
Updates for better JLCPCB processing. Version is now 1.1
</commit_message>
<xml_diff>
--- a/rp2350b-launchpad-PCB-top-pos.xlsx
+++ b/rp2350b-launchpad-PCB-top-pos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="243">
   <si>
     <t xml:space="preserve">Designator</t>
   </si>
@@ -365,6 +365,9 @@
   </si>
   <si>
     <t xml:space="preserve">10.990000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">65.024000</t>
   </si>
   <si>
     <t xml:space="preserve">L2</t>
@@ -873,11 +876,11 @@
   </sheetPr>
   <dimension ref="A1:I107"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2:E107"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A83" activeCellId="0" sqref="A83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.44"/>
@@ -1741,7 +1744,7 @@
         <v>114</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="D48" s="0" t="s">
         <v>8</v>
@@ -1753,13 +1756,13 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D49" s="0" t="s">
         <v>8</v>
@@ -1771,13 +1774,13 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B50" s="0" t="s">
         <v>100</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D50" s="0" t="s">
         <v>8</v>
@@ -1789,10 +1792,10 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C51" s="0" t="s">
         <v>7</v>
@@ -1807,7 +1810,7 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B52" s="0" t="s">
         <v>100</v>
@@ -1825,7 +1828,7 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B53" s="0" t="s">
         <v>100</v>
@@ -1843,10 +1846,10 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C54" s="0" t="s">
         <v>103</v>
@@ -1861,13 +1864,13 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D55" s="0" t="s">
         <v>8</v>
@@ -1879,13 +1882,13 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D56" s="0" t="s">
         <v>8</v>
@@ -1897,13 +1900,13 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D57" s="0" t="s">
         <v>8</v>
@@ -1915,10 +1918,10 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C58" s="0" t="s">
         <v>31</v>
@@ -1933,7 +1936,7 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B59" s="0" t="s">
         <v>25</v>
@@ -1951,10 +1954,10 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C60" s="0" t="s">
         <v>31</v>
@@ -1969,7 +1972,7 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B61" s="0" t="s">
         <v>33</v>
@@ -1987,10 +1990,10 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C62" s="0" t="s">
         <v>19</v>
@@ -2005,10 +2008,10 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C63" s="0" t="s">
         <v>105</v>
@@ -2023,10 +2026,10 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C64" s="0" t="s">
         <v>107</v>
@@ -2041,10 +2044,10 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C65" s="0" t="s">
         <v>109</v>
@@ -2059,13 +2062,13 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D66" s="0" t="s">
         <v>8</v>
@@ -2077,10 +2080,10 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C67" s="0" t="s">
         <v>85</v>
@@ -2095,13 +2098,13 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D68" s="0" t="s">
         <v>8</v>
@@ -2113,13 +2116,13 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="B69" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="C69" s="0" t="s">
         <v>151</v>
-      </c>
-      <c r="B69" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="C69" s="0" t="s">
-        <v>150</v>
       </c>
       <c r="D69" s="0" t="s">
         <v>8</v>
@@ -2131,7 +2134,7 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B70" s="0" t="s">
         <v>67</v>
@@ -2149,13 +2152,13 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D71" s="0" t="s">
         <v>8</v>
@@ -2167,13 +2170,13 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D72" s="0" t="s">
         <v>8</v>
@@ -2185,7 +2188,7 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B73" s="0" t="s">
         <v>84</v>
@@ -2203,10 +2206,10 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C74" s="0" t="s">
         <v>58</v>
@@ -2221,13 +2224,13 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D75" s="0" t="s">
         <v>8</v>
@@ -2239,13 +2242,13 @@
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D76" s="0" t="s">
         <v>8</v>
@@ -2257,13 +2260,13 @@
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B77" s="0" t="s">
         <v>84</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D77" s="0" t="s">
         <v>8</v>
@@ -2275,13 +2278,13 @@
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D78" s="0" t="s">
         <v>8</v>
@@ -2293,13 +2296,13 @@
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B79" s="0" t="s">
         <v>84</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D79" s="0" t="s">
         <v>8</v>
@@ -2311,13 +2314,13 @@
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D80" s="0" t="s">
         <v>8</v>
@@ -2329,13 +2332,13 @@
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="B81" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="C81" s="0" t="s">
         <v>179</v>
-      </c>
-      <c r="B81" s="0" t="s">
-        <v>180</v>
-      </c>
-      <c r="C81" s="0" t="s">
-        <v>178</v>
       </c>
       <c r="D81" s="0" t="s">
         <v>8</v>
@@ -2347,10 +2350,10 @@
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C82" s="0" t="s">
         <v>112</v>
@@ -2365,13 +2368,13 @@
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D83" s="0" t="s">
         <v>8</v>
@@ -2383,13 +2386,13 @@
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D84" s="0" t="s">
         <v>8</v>
@@ -2401,13 +2404,13 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D85" s="0" t="s">
         <v>8</v>
@@ -2419,13 +2422,13 @@
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D86" s="0" t="s">
         <v>8</v>
@@ -2437,13 +2440,13 @@
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D87" s="0" t="s">
         <v>8</v>
@@ -2455,13 +2458,13 @@
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D88" s="0" t="s">
         <v>8</v>
@@ -2473,13 +2476,13 @@
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D89" s="0" t="s">
         <v>8</v>
@@ -2491,13 +2494,13 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D90" s="0" t="s">
         <v>8</v>
@@ -2509,13 +2512,13 @@
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B91" s="0" t="s">
         <v>82</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D91" s="0" t="s">
         <v>8</v>
@@ -2527,13 +2530,13 @@
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D92" s="0" t="s">
         <v>8</v>
@@ -2545,13 +2548,13 @@
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D93" s="0" t="s">
         <v>8</v>
@@ -2563,13 +2566,13 @@
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D94" s="0" t="s">
         <v>8</v>
@@ -2577,17 +2580,16 @@
       <c r="E94" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="I94" s="1"/>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D95" s="0" t="s">
         <v>8</v>
@@ -2595,14 +2597,13 @@
       <c r="E95" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="I95" s="1"/>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C96" s="0" t="s">
         <v>112</v>
@@ -2613,14 +2614,13 @@
       <c r="E96" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="I96" s="1"/>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C97" s="0" t="s">
         <v>112</v>
@@ -2631,14 +2631,13 @@
       <c r="E97" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="I97" s="1"/>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B98" s="0" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C98" s="0" t="s">
         <v>112</v>
@@ -2649,14 +2648,13 @@
       <c r="E98" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="I98" s="1"/>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B99" s="0" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C99" s="0" t="s">
         <v>112</v>
@@ -2667,14 +2665,13 @@
       <c r="E99" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="I99" s="1"/>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B100" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C100" s="0" t="s">
         <v>112</v>
@@ -2685,14 +2682,13 @@
       <c r="E100" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="I100" s="1"/>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B101" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C101" s="0" t="s">
         <v>112</v>
@@ -2703,14 +2699,13 @@
       <c r="E101" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="I101" s="1"/>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B102" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C102" s="0" t="s">
         <v>112</v>
@@ -2721,11 +2716,10 @@
       <c r="E102" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="I102" s="1"/>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B103" s="0" t="s">
         <v>27</v>
@@ -2739,17 +2733,16 @@
       <c r="E103" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="I103" s="1"/>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B104" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C104" s="0" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D104" s="0" t="s">
         <v>8</v>
@@ -2757,17 +2750,16 @@
       <c r="E104" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="I104" s="1"/>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B105" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C105" s="0" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D105" s="0" t="s">
         <v>8</v>
@@ -2775,17 +2767,16 @@
       <c r="E105" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="I105" s="1"/>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B106" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C106" s="0" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D106" s="0" t="s">
         <v>8</v>
@@ -2793,17 +2784,16 @@
       <c r="E106" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="I106" s="1"/>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B107" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C107" s="0" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D107" s="0" t="s">
         <v>8</v>
@@ -2811,7 +2801,6 @@
       <c r="E107" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="I107" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>